<commit_message>
adding test cases to plan tx
</commit_message>
<xml_diff>
--- a/spec/test_data/rating_factors.xlsx
+++ b/spec/test_data/rating_factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nisanthyaganti/Documents/quoting_tool/spec/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F62398C-F0D8-FC48-8684-9E86767809C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4627EA-C3AE-C74E-9667-BFAC962A2FE7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard Industry Code Factors" sheetId="3" r:id="rId1"/>
@@ -3758,7 +3758,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:M1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -18905,7 +18905,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B60" sqref="A8:B60"/>
     </sheetView>
   </sheetViews>
@@ -21385,7 +21385,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>